<commit_message>
I try to do API function for director
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="a1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="A2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="A1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="a11" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,75 +466,6 @@
         <is>
           <t>Created</t>
         </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>a1</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>3</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>113</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>a1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>113</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>a1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -548,7 +479,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -583,29 +514,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>A2</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Finally excel download is fixed
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -8,8 +8,8 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="A1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="a11" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="a1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="A11" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,171 @@
         <is>
           <t>Created</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -479,7 +644,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +679,171 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>A1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>a1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Finally excel creation is fixed
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,193 +444,18 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Id</t>
+          <t>model</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Serial</t>
+          <t>version</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Model</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Version</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Created</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>a1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>a1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>a1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
+          <t>created</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -644,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -655,27 +480,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Id</t>
+          <t>model</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Serial</t>
+          <t>version</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Model</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Version</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Created</t>
+          <t>created</t>
         </is>
       </c>
     </row>
@@ -687,161 +502,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>21</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>A1</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>a1</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>a1</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>